<commit_message>
Last Updated on 4/22
Last Updated on 4/22
</commit_message>
<xml_diff>
--- a/doc/Plan.xlsx
+++ b/doc/Plan.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijinkp/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AtulHome\Desktop\M Tech\Forth Sem\Classes\Deep Learning\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="52">
   <si>
     <t>Phase 1 (Running the data without fine tuning in the existing architectures) :</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Phase 2 (Fine tuning existing architectures to suit our datasets for better accuracy):</t>
   </si>
   <si>
-    <t>Phase 3 :</t>
-  </si>
-  <si>
     <t>Task/Milestone</t>
   </si>
   <si>
@@ -56,18 +53,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Try to fine tune image classification layer(Resnet/VGG) to suit our dataset using transfer learning.</t>
-  </si>
-  <si>
-    <t>Fine tuned models needs to be incorporated in SSD/Faster R-CNN/Mask R-CNN and analyse accuracy.</t>
-  </si>
-  <si>
-    <t>Architecture enhancements. (Not clear what to do at this point).</t>
-  </si>
-  <si>
-    <t>Running one complex dataset (Stanford drone data).</t>
-  </si>
-  <si>
     <t>Understand SSD Architecture</t>
   </si>
   <si>
@@ -90,9 +75,6 @@
   </si>
   <si>
     <t>Milestone 1 complete</t>
-  </si>
-  <si>
-    <t>Milestone 2 complete</t>
   </si>
   <si>
     <t>Assigned To</t>
@@ -150,14 +132,68 @@
     <t>To Be Started</t>
   </si>
   <si>
-    <t>Running code on py 3.6</t>
+    <t>Understand next steps in phase2 : Meeting with joseph</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Train and test on one dataset. Evaluate the results with mAP</t>
+  </si>
+  <si>
+    <t>Pascal VOC Annotation change for 2 class model</t>
+  </si>
+  <si>
+    <t>Train and Test VOC 2 Class Model</t>
+  </si>
+  <si>
+    <t>Prepare Report for submission</t>
+  </si>
+  <si>
+    <t>Vijin, Chandra, Atul</t>
+  </si>
+  <si>
+    <t>Evaluation Faster RCNN with Vijin's Method</t>
+  </si>
+  <si>
+    <t>Chang SSD for 2 class model (Train and Test)</t>
+  </si>
+  <si>
+    <t>Change Faster R-CNN for 2 class model (Train and Test)</t>
+  </si>
+  <si>
+    <t>Change RFCN for 2 class model (Train and Test)</t>
+  </si>
+  <si>
+    <t>Error Fixed (RFCN)</t>
+  </si>
+  <si>
+    <t>Evaluation RFCN with Vijin's Method</t>
+  </si>
+  <si>
+    <t>Train and Test Mini Drone Class Model</t>
+  </si>
+  <si>
+    <t>Test Mini drone with VOC train Model</t>
+  </si>
+  <si>
+    <t>Test Okutama with VOC train Model</t>
+  </si>
+  <si>
+    <t>Train and Test Okutama Class Model</t>
+  </si>
+  <si>
+    <t>Finalize the model</t>
+  </si>
+  <si>
+    <t>To be started</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +242,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -242,10 +301,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2" readingOrder="1"/>
@@ -293,13 +354,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,52 +648,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="49.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="49.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -636,28 +704,28 @@
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H3" s="19"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="11">
@@ -667,20 +735,20 @@
         <v>43169</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H4" s="19"/>
-      <c r="I4" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="11">
@@ -689,21 +757,19 @@
       <c r="F5" s="11">
         <v>43177</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="23">
-        <v>43189</v>
-      </c>
-      <c r="I5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="11">
@@ -713,18 +779,18 @@
         <v>43177</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H6" s="19"/>
-      <c r="I6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="23"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="11">
@@ -734,18 +800,18 @@
         <v>43184</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H7" s="19"/>
-      <c r="I7" s="21"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7" s="23"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>22</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="11">
@@ -755,20 +821,20 @@
         <v>43177</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="11">
@@ -777,23 +843,21 @@
       <c r="F9" s="11">
         <v>43177</v>
       </c>
-      <c r="G9" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="23">
-        <v>43189</v>
-      </c>
+      <c r="G9" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="19"/>
       <c r="I9" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="11">
@@ -803,14 +867,14 @@
         <v>43177</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="8"/>
       <c r="C11" s="17"/>
@@ -821,10 +885,10 @@
       <c r="H11" s="19"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="9"/>
@@ -833,16 +897,16 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="20" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="11">
@@ -851,19 +915,23 @@
       <c r="F13" s="11">
         <v>43191</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="11">
+        <v>43200</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="11">
@@ -872,19 +940,21 @@
       <c r="F14" s="11">
         <v>43191</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G14" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="11">
+        <v>43212</v>
+      </c>
+      <c r="I14" s="24"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="20" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="11">
@@ -893,59 +963,69 @@
       <c r="F15" s="11">
         <v>43191</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15">
+      <c r="G15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="11">
+        <v>43200</v>
+      </c>
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="11">
+        <v>43198</v>
+      </c>
+      <c r="F17" s="11">
+        <v>43200</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="22">
+        <v>43202</v>
+      </c>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15">
         <v>43190</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F18" s="15">
         <v>43190</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="16"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="2" t="s">
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" ht="26" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" ht="26" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="6"/>
@@ -955,90 +1035,458 @@
       <c r="H19" s="6"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15">
-        <v>43205</v>
-      </c>
-      <c r="F20" s="15">
-        <v>43205</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="16"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="17"/>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="25">
+        <v>43212</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="F22" s="25">
+        <v>43214</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="17"/>
+        <v>47</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>16</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="F23" s="25">
+        <v>43219</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15">
-        <v>43205</v>
-      </c>
-      <c r="F24" s="15">
-        <v>43205</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C25" s="17"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="25">
+        <v>43219</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="25">
+        <v>43220</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="25">
+        <v>43212</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="25">
+        <v>43214</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="25">
+        <v>43215</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="25">
+        <v>43219</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="25">
+        <v>43219</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="25">
+        <v>43220</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="25">
+        <v>43220</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="25">
+        <v>43212</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="25">
+        <v>43214</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="25">
+        <v>43219</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="25">
+        <v>43219</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="25">
+        <v>43220</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="6"/>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="25">
+        <v>43220</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" s="6"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>39</v>
       </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="25">
+        <v>43214</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="14"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15">
+        <v>43221</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H43" s="14"/>
+      <c r="I43" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I13:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates as on 20180424
</commit_message>
<xml_diff>
--- a/doc/Plan.xlsx
+++ b/doc/Plan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AtulHome\Desktop\M Tech\Forth Sem\Classes\Deep Learning\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cananthapatn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="52">
   <si>
     <t>Phase 1 (Running the data without fine tuning in the existing architectures) :</t>
   </si>
@@ -129,9 +129,6 @@
     <t>R-FCN</t>
   </si>
   <si>
-    <t>To Be Started</t>
-  </si>
-  <si>
     <t>Understand next steps in phase2 : Meeting with joseph</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>To be started</t>
+  </si>
+  <si>
+    <t>Train Complete</t>
   </si>
 </sst>
 </file>
@@ -354,17 +354,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -650,21 +650,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="49.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="49.44140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -691,7 +693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -704,7 +706,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="8" t="s">
         <v>24</v>
@@ -719,7 +721,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="8" t="s">
         <v>7</v>
@@ -738,11 +740,11 @@
         <v>25</v>
       </c>
       <c r="H4" s="19"/>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -761,9 +763,9 @@
         <v>25</v>
       </c>
       <c r="H5" s="19"/>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="8" t="s">
         <v>9</v>
@@ -782,9 +784,9 @@
         <v>27</v>
       </c>
       <c r="H6" s="19"/>
-      <c r="I6" s="23"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="8" t="s">
         <v>28</v>
@@ -803,9 +805,9 @@
         <v>25</v>
       </c>
       <c r="H7" s="19"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="8" t="s">
         <v>11</v>
@@ -828,7 +830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="8" t="s">
         <v>12</v>
@@ -851,7 +853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="8" t="s">
         <v>13</v>
@@ -874,7 +876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="8"/>
       <c r="C11" s="17"/>
@@ -885,7 +887,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="8" t="s">
         <v>19</v>
@@ -900,7 +902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="20" t="s">
         <v>29</v>
@@ -921,11 +923,11 @@
       <c r="H13" s="11">
         <v>43200</v>
       </c>
-      <c r="I13" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="20" t="s">
         <v>30</v>
@@ -940,15 +942,15 @@
       <c r="F14" s="11">
         <v>43191</v>
       </c>
-      <c r="G14" s="21" t="s">
-        <v>32</v>
+      <c r="G14" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="H14" s="11">
         <v>43212</v>
       </c>
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="20" t="s">
         <v>31</v>
@@ -969,9 +971,9 @@
       <c r="H15" s="11">
         <v>43200</v>
       </c>
-      <c r="I15" s="24"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="20"/>
       <c r="C16" s="17"/>
@@ -982,13 +984,13 @@
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>34</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="11">
@@ -1000,12 +1002,12 @@
       <c r="G17" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
         <v>43202</v>
       </c>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
         <v>14</v>
@@ -1022,7 +1024,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="2" t="s">
         <v>1</v>
@@ -1035,10 +1037,10 @@
       <c r="H19" s="6"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>16</v>
@@ -1052,36 +1054,36 @@
       <c r="H20" s="6"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="25">
+      <c r="F21" s="22">
         <v>43212</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>26</v>
+      <c r="G21" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="25">
+      <c r="F22" s="22">
         <v>43214</v>
       </c>
       <c r="G22" s="6" t="s">
@@ -1090,17 +1092,17 @@
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="25">
+      <c r="F23" s="22">
         <v>43219</v>
       </c>
       <c r="G23" s="6" t="s">
@@ -1109,17 +1111,17 @@
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="25">
+      <c r="F24" s="22">
         <v>43219</v>
       </c>
       <c r="G24" s="6" t="s">
@@ -1128,34 +1130,34 @@
       <c r="H24" s="6"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
-      <c r="F25" s="25"/>
+      <c r="F25" s="22"/>
       <c r="G25" s="19" t="s">
         <v>25</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="25">
+      <c r="F26" s="22">
         <v>43220</v>
       </c>
       <c r="G26" s="6" t="s">
@@ -1164,55 +1166,55 @@
       <c r="H26" s="6"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="25">
+      <c r="F27" s="22">
         <v>43212</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
-      <c r="F28" s="25">
+      <c r="F28" s="22">
         <v>43214</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>26</v>
+      <c r="G28" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
-      <c r="F29" s="25">
+      <c r="F29" s="22">
         <v>43215</v>
       </c>
       <c r="G29" s="6" t="s">
@@ -1221,17 +1223,17 @@
       <c r="H29" s="6"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
-      <c r="F30" s="25">
+      <c r="F30" s="22">
         <v>43219</v>
       </c>
       <c r="G30" s="6" t="s">
@@ -1240,17 +1242,17 @@
       <c r="H30" s="6"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="25">
+      <c r="F31" s="22">
         <v>43219</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1259,36 +1261,38 @@
       <c r="H31" s="6"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="25">
+      <c r="F32" s="22">
         <v>43220</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="25">
+      <c r="F33" s="22">
         <v>43220</v>
       </c>
       <c r="G33" s="6" t="s">
@@ -1297,10 +1301,10 @@
       <c r="H33" s="6"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>18</v>
@@ -1314,10 +1318,10 @@
       <c r="H34" s="6"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>18</v>
@@ -1331,55 +1335,55 @@
       <c r="H35" s="6"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="25">
+      <c r="F36" s="22">
         <v>43212</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>26</v>
+      <c r="G36" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="25">
+      <c r="F37" s="22">
         <v>43214</v>
       </c>
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="25">
+      <c r="F38" s="22">
         <v>43219</v>
       </c>
       <c r="G38" s="6" t="s">
@@ -1388,17 +1392,17 @@
       <c r="H38" s="6"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="25">
+      <c r="F39" s="22">
         <v>43219</v>
       </c>
       <c r="G39" s="6" t="s">
@@ -1407,36 +1411,38 @@
       <c r="H39" s="6"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="25">
+      <c r="F40" s="22">
         <v>43220</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H40" s="6"/>
+      <c r="H40" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="25">
+      <c r="F41" s="22">
         <v>43220</v>
       </c>
       <c r="G41" s="6" t="s">
@@ -1445,32 +1451,32 @@
       <c r="H41" s="6"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="25">
+      <c r="F42" s="22">
         <v>43214</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="12"/>
       <c r="B43" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>39</v>
+        <v>49</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="15"/>
@@ -1478,7 +1484,7 @@
         <v>43221</v>
       </c>
       <c r="G43" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H43" s="14"/>
       <c r="I43" s="16"/>

</xml_diff>